<commit_message>
Ajout Creation PDF + Code BAr
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\phpexcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetDDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8760605F-5C1F-4D0E-9B60-9B699DD4E851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEDB194-0390-4EBA-AADB-2417C6690E2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="1095" windowWidth="10620" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1755" yWindow="6510" windowWidth="10875" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -34,16 +34,16 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Iphone 8TPU</t>
-  </si>
-  <si>
-    <t>Iphone 8PC</t>
-  </si>
-  <si>
-    <t>Visu/Plastique/Iphone8/*</t>
-  </si>
-  <si>
     <t>Visu/Silicone/Iphone8/*</t>
+  </si>
+  <si>
+    <t>Iphone6TPU</t>
+  </si>
+  <si>
+    <t>Iphone8TPU</t>
+  </si>
+  <si>
+    <t>Visu/Silicone/Iphone6/*</t>
   </si>
 </sst>
 </file>
@@ -385,13 +385,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="66.7109375" customWidth="1"/>
@@ -413,13 +413,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>1950</v>
+        <v>518</v>
       </c>
       <c r="C2">
-        <v>500</v>
+        <v>238</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -427,16 +427,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>1620</v>
+        <v>538</v>
       </c>
       <c r="C3">
-        <v>600</v>
+        <v>238</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification Design et Ajout page de visualisation
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetDDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE9F23C-6510-48F3-916B-7D80B00D738D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAF1ED5-BB99-426F-87CC-1AFC98347DFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Téléphone</t>
   </si>
@@ -39,54 +39,12 @@
     <t>Largeur</t>
   </si>
   <si>
-    <t>Iphone6</t>
-  </si>
-  <si>
-    <t>Iphone8</t>
-  </si>
-  <si>
-    <t>Iphone11 6.1</t>
-  </si>
-  <si>
-    <t>Iphone11 Pro 5.8</t>
-  </si>
-  <si>
-    <t>Iphone11 Pro Max 6.5</t>
-  </si>
-  <si>
-    <t>IphoneX</t>
-  </si>
-  <si>
-    <t>IphoneXr</t>
-  </si>
-  <si>
-    <t>IphoneXS MAX</t>
-  </si>
-  <si>
-    <t>Iphone4</t>
-  </si>
-  <si>
-    <t>Iphone5</t>
-  </si>
-  <si>
-    <t>Iphone5C</t>
-  </si>
-  <si>
-    <t>Iphone6 Plus</t>
-  </si>
-  <si>
     <t>Iphone 7</t>
   </si>
   <si>
-    <t>Iphone 7 Plus</t>
-  </si>
-  <si>
     <t>Ipod Touch 6</t>
   </si>
   <si>
-    <t>Galaxy S6 Edge Plus</t>
-  </si>
-  <si>
     <t>Galaxy S6</t>
   </si>
   <si>
@@ -102,24 +60,15 @@
     <t>Galaxy S8</t>
   </si>
   <si>
-    <t>Galaxy S8 Plus</t>
-  </si>
-  <si>
     <t>Galaxy S9</t>
   </si>
   <si>
-    <t>Galaxy S9 Plus</t>
-  </si>
-  <si>
     <t>Galaxy S10</t>
   </si>
   <si>
     <t>Galaxy S10E</t>
   </si>
   <si>
-    <t>Galaxy S10 Plus</t>
-  </si>
-  <si>
     <t>Galaxy A3</t>
   </si>
   <si>
@@ -141,9 +90,6 @@
     <t>Galaxy A6 2018</t>
   </si>
   <si>
-    <t>Galaxy A6 PLUS 2018</t>
-  </si>
-  <si>
     <t>Galaxy A7</t>
   </si>
   <si>
@@ -162,9 +108,6 @@
     <t>Galaxy A8 2018</t>
   </si>
   <si>
-    <t>Galaxy A8 Plus 2018</t>
-  </si>
-  <si>
     <t>Galaxy A9</t>
   </si>
   <si>
@@ -246,45 +189,24 @@
     <t>P8</t>
   </si>
   <si>
-    <t>P8 Lite</t>
-  </si>
-  <si>
-    <t>P8 Lite 2017</t>
-  </si>
-  <si>
     <t>P9</t>
   </si>
   <si>
-    <t>P9 Lite</t>
-  </si>
-  <si>
-    <t>P9 Plus</t>
-  </si>
-  <si>
     <t xml:space="preserve">P10 </t>
   </si>
   <si>
-    <t>P10 Lite</t>
-  </si>
-  <si>
     <t>P20</t>
   </si>
   <si>
     <t>P20 Pro</t>
   </si>
   <si>
-    <t>P20 Lite</t>
-  </si>
-  <si>
     <t>P30</t>
   </si>
   <si>
     <t>P30 Pro</t>
   </si>
   <si>
-    <t>P30 Lite</t>
-  </si>
-  <si>
     <t>Psmart</t>
   </si>
   <si>
@@ -300,18 +222,12 @@
     <t>Mate 10 Pro</t>
   </si>
   <si>
-    <t>Mate 10 Lite</t>
-  </si>
-  <si>
     <t>Mate 20</t>
   </si>
   <si>
     <t>Mate 20 Pro</t>
   </si>
   <si>
-    <t>Mate 20 Lite</t>
-  </si>
-  <si>
     <t>Honor 6</t>
   </si>
   <si>
@@ -330,9 +246,6 @@
     <t>Honor 10</t>
   </si>
   <si>
-    <t>Honor 10 Lite</t>
-  </si>
-  <si>
     <t>Y5 2019</t>
   </si>
   <si>
@@ -391,6 +304,90 @@
   </si>
   <si>
     <t>XZ3</t>
+  </si>
+  <si>
+    <t>Iphone 7 +</t>
+  </si>
+  <si>
+    <t>Galaxy S6 Edge +</t>
+  </si>
+  <si>
+    <t>Galaxy S8 +</t>
+  </si>
+  <si>
+    <t>Galaxy S9 +</t>
+  </si>
+  <si>
+    <t>Galaxy S10 +</t>
+  </si>
+  <si>
+    <t>Galaxy A6 + 2018</t>
+  </si>
+  <si>
+    <t>Galaxy A8 + 2018</t>
+  </si>
+  <si>
+    <t>P9 +</t>
+  </si>
+  <si>
+    <t>P8 LTE</t>
+  </si>
+  <si>
+    <t>P8 LTE 2017</t>
+  </si>
+  <si>
+    <t>P9 LTE</t>
+  </si>
+  <si>
+    <t>P10 LTE</t>
+  </si>
+  <si>
+    <t>P20 LTE</t>
+  </si>
+  <si>
+    <t>P30 LTE</t>
+  </si>
+  <si>
+    <t>Mate 10 LTE</t>
+  </si>
+  <si>
+    <t>Mate 20 LTE</t>
+  </si>
+  <si>
+    <t>Honor 10 LTE</t>
+  </si>
+  <si>
+    <t>Iphone 11 6.1</t>
+  </si>
+  <si>
+    <t>Iphone 11 Pro</t>
+  </si>
+  <si>
+    <t>Iphone 11 Pro Max</t>
+  </si>
+  <si>
+    <t>Iphone X</t>
+  </si>
+  <si>
+    <t>Iphone Xr</t>
+  </si>
+  <si>
+    <t>Iphone XS MAX</t>
+  </si>
+  <si>
+    <t>Iphone 4</t>
+  </si>
+  <si>
+    <t>Iphone 5</t>
+  </si>
+  <si>
+    <t>Iphone 5C</t>
+  </si>
+  <si>
+    <t>Iphone 6</t>
+  </si>
+  <si>
+    <t>Iphone 6 +</t>
   </si>
 </sst>
 </file>
@@ -811,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H119"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +822,7 @@
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -836,9 +833,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="B2">
         <v>145</v>
@@ -847,9 +844,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="B3">
         <v>139</v>
@@ -858,9 +855,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="B4">
         <v>151</v>
@@ -869,9 +866,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="B5">
         <v>136</v>
@@ -880,9 +877,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="B6">
         <v>142</v>
@@ -890,19 +887,10 @@
       <c r="C6">
         <v>67</v>
       </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>510</v>
-      </c>
-      <c r="H6">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="B7">
         <v>151</v>
@@ -910,19 +898,10 @@
       <c r="C7">
         <v>69</v>
       </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>680</v>
-      </c>
-      <c r="H7">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="B8">
         <v>115</v>
@@ -931,9 +910,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>116</v>
       </c>
       <c r="B9">
         <v>123</v>
@@ -942,9 +921,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
       <c r="B10">
         <v>120</v>
@@ -953,9 +932,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="B11">
         <v>132</v>
@@ -964,9 +943,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="B12">
         <v>147</v>
@@ -975,9 +954,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>130</v>
@@ -986,9 +965,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="B14">
         <v>151</v>
@@ -997,9 +976,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>117</v>
@@ -1008,9 +987,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>134</v>
@@ -1021,7 +1000,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>135</v>
@@ -1033,7 +1012,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="B18">
         <v>150</v>
@@ -1044,7 +1023,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>132</v>
@@ -1055,7 +1034,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>141</v>
@@ -1066,7 +1045,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <v>140</v>
@@ -1077,7 +1056,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="B22">
         <v>151</v>
@@ -1088,7 +1067,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>140</v>
@@ -1099,7 +1078,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B24">
         <v>149</v>
@@ -1110,7 +1089,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B25">
         <v>140</v>
@@ -1121,7 +1100,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B26">
         <v>130</v>
@@ -1132,7 +1111,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="B27">
         <v>148</v>
@@ -1143,7 +1122,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B28">
         <v>120</v>
@@ -1154,7 +1133,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B29">
         <v>130</v>
@@ -1165,7 +1144,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B30">
         <v>128</v>
@@ -1176,7 +1155,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B31">
         <v>1310</v>
@@ -1187,7 +1166,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B32">
         <v>139</v>
@@ -1198,7 +1177,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B33">
         <v>138</v>
@@ -1209,7 +1188,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B34">
         <v>138</v>
@@ -1220,7 +1199,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="B35">
         <v>148</v>
@@ -1231,7 +1210,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B36">
         <v>141</v>
@@ -1242,7 +1221,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B37">
         <v>145</v>
@@ -1253,7 +1232,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B38">
         <v>149</v>
@@ -1264,7 +1243,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B39">
         <v>150</v>
@@ -1275,7 +1254,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B40">
         <v>150</v>
@@ -1286,7 +1265,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B41">
         <v>141</v>
@@ -1297,7 +1276,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="B42">
         <v>151</v>
@@ -1308,7 +1287,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B43">
         <v>155</v>
@@ -1319,7 +1298,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B44">
         <v>129</v>
@@ -1330,7 +1309,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B45">
         <v>128</v>
@@ -1341,7 +1320,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B46">
         <v>136</v>
@@ -1352,7 +1331,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B47">
         <v>129</v>
@@ -1363,7 +1342,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B48">
         <v>132</v>
@@ -1374,7 +1353,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B49">
         <v>138</v>
@@ -1385,7 +1364,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B50">
         <v>137</v>
@@ -1396,7 +1375,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B51">
         <v>152</v>
@@ -1407,7 +1386,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B52">
         <v>144</v>
@@ -1418,7 +1397,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B53">
         <v>148</v>
@@ -1429,7 +1408,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B54">
         <v>146</v>
@@ -1440,7 +1419,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B55">
         <v>150</v>
@@ -1451,7 +1430,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B56">
         <v>154</v>
@@ -1462,7 +1441,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B57">
         <v>153</v>
@@ -1473,7 +1452,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B58">
         <v>147</v>
@@ -1484,7 +1463,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B59">
         <v>157</v>
@@ -1495,7 +1474,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B60">
         <v>134</v>
@@ -1506,7 +1485,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B61">
         <v>147</v>
@@ -1517,7 +1496,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B62">
         <v>147</v>
@@ -1528,7 +1507,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B63">
         <v>159</v>
@@ -1539,7 +1518,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B64">
         <v>159</v>
@@ -1550,7 +1529,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B65">
         <v>147</v>
@@ -1561,7 +1540,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B66">
         <v>140</v>
@@ -1572,7 +1551,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B67">
         <v>157</v>
@@ -1583,7 +1562,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B68">
         <v>155</v>
@@ -1594,7 +1573,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B69">
         <v>139</v>
@@ -1605,7 +1584,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B70">
         <v>139</v>
@@ -1616,7 +1595,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B71">
         <v>141</v>
@@ -1627,7 +1606,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B72">
         <v>134</v>
@@ -1638,7 +1617,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="B73">
         <v>139</v>
@@ -1649,7 +1628,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="B74">
         <v>139</v>
@@ -1660,7 +1639,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B75">
         <v>138</v>
@@ -1671,7 +1650,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="B76">
         <v>139</v>
@@ -1682,7 +1661,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="B77">
         <v>140</v>
@@ -1693,7 +1672,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="B78">
         <v>148</v>
@@ -1704,7 +1683,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="B79">
         <v>142</v>
@@ -1715,7 +1694,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B80">
         <v>139</v>
@@ -1726,7 +1705,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B81">
         <v>144</v>
@@ -1737,7 +1716,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B82">
         <v>142</v>
@@ -1748,7 +1727,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B83">
         <v>139</v>
@@ -1759,7 +1738,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="B84">
         <v>149</v>
@@ -1770,7 +1749,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="B85">
         <v>150</v>
@@ -1781,7 +1760,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B86">
         <v>140</v>
@@ -1792,7 +1771,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="B87">
         <v>146</v>
@@ -1803,7 +1782,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B88">
         <v>148</v>
@@ -1814,7 +1793,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="B89">
         <v>151</v>
@@ -1825,7 +1804,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="B90">
         <v>148</v>
@@ -1836,7 +1815,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B91">
         <v>150</v>
@@ -1847,7 +1826,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="B92">
         <v>135</v>
@@ -1858,7 +1837,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B93">
         <v>135</v>
@@ -1869,7 +1848,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B94">
         <v>138</v>
@@ -1880,7 +1859,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B95">
         <v>152</v>
@@ -1891,7 +1870,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="B96">
         <v>138</v>
@@ -1902,7 +1881,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="B97">
         <v>140</v>
@@ -1913,7 +1892,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B98">
         <v>150</v>
@@ -1924,7 +1903,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="B99">
         <v>140</v>
@@ -1935,7 +1914,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B100">
         <v>141</v>
@@ -1946,7 +1925,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B101">
         <v>153</v>
@@ -1957,7 +1936,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="B102">
         <v>155</v>
@@ -1968,7 +1947,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B103">
         <v>145</v>
@@ -1979,7 +1958,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="B104">
         <v>145</v>
@@ -1990,7 +1969,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="B105">
         <v>145</v>
@@ -2001,7 +1980,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B106">
         <v>142</v>
@@ -2012,7 +1991,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="B107">
         <v>123</v>
@@ -2023,7 +2002,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B108">
         <v>160</v>
@@ -2034,7 +2013,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="B109">
         <v>138</v>
@@ -2045,7 +2024,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B110">
         <v>138</v>
@@ -2056,7 +2035,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="B111">
         <v>160</v>
@@ -2067,7 +2046,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B112">
         <v>141</v>
@@ -2078,7 +2057,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="B113">
         <v>160</v>
@@ -2089,7 +2068,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="B114">
         <v>160</v>
@@ -2100,7 +2079,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B115">
         <v>143</v>
@@ -2111,7 +2090,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="B116">
         <v>145</v>
@@ -2122,7 +2101,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="B117">
         <v>133</v>
@@ -2133,7 +2112,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="B118">
         <v>141</v>

</xml_diff>

<commit_message>
Ajout chaine de caractere inversé + DPI des images
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetDDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D769D30-1826-4393-B34E-54EC261457FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5577B1E-DD7E-4C15-B951-74654106A8BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="183">
   <si>
     <t>Téléphone</t>
   </si>
@@ -387,14 +387,203 @@
     <t>Iphone 6 +</t>
   </si>
   <si>
-    <t>Iphone6</t>
+    <t>Iphone 6</t>
+  </si>
+  <si>
+    <t>OnePlus 5</t>
+  </si>
+  <si>
+    <t>OnePlus 5T</t>
+  </si>
+  <si>
+    <t>OnePlus 6</t>
+  </si>
+  <si>
+    <t>OnePlus 6T</t>
+  </si>
+  <si>
+    <t>OnePlus 7</t>
+  </si>
+  <si>
+    <t>OnePlus 7 PRO</t>
+  </si>
+  <si>
+    <t>ONe Plus X</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi 6</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi 6X</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi 7 / Mi 8</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi 8 lite</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi 8 Pro</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi 9 / Mi 9 Pro</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi A2</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi A2 lite</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi Mix 2</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi Mix 2S</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi Mix 3</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi Max 2</t>
+  </si>
+  <si>
+    <t>Xiaomi 5 Plus</t>
+  </si>
+  <si>
+    <t>Xiaomi 6</t>
+  </si>
+  <si>
+    <t>Xiaomi 6A</t>
+  </si>
+  <si>
+    <t>Xiaomi 6 Pro</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 5 / Note 5 PRO</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 6 / Note 6 PRO</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 7 / Note 7 PRO</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 8</t>
+  </si>
+  <si>
+    <t>Zenfone 2</t>
+  </si>
+  <si>
+    <t>Zenfone 3</t>
+  </si>
+  <si>
+    <t>Zenfone 3 MAX</t>
+  </si>
+  <si>
+    <t>Zenfone 4 MAX</t>
+  </si>
+  <si>
+    <t>Zenfone 5</t>
+  </si>
+  <si>
+    <t>Zenfone 5 Lite</t>
+  </si>
+  <si>
+    <t>Zenfone 5Z</t>
+  </si>
+  <si>
+    <t>Zenfone Go</t>
+  </si>
+  <si>
+    <t>Zenfone Max Plus M1</t>
+  </si>
+  <si>
+    <t>Zenfone Max Pro M1</t>
+  </si>
+  <si>
+    <t>Selfie</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>Motorola ONE</t>
+  </si>
+  <si>
+    <t>Nokia 3</t>
+  </si>
+  <si>
+    <t>Nokia 6 2018</t>
+  </si>
+  <si>
+    <t>Nokia 7 Plus</t>
+  </si>
+  <si>
+    <t>Nokia 8</t>
+  </si>
+  <si>
+    <t>Lumia 520</t>
+  </si>
+  <si>
+    <t>Lumia 610</t>
+  </si>
+  <si>
+    <t>Lumia 620</t>
+  </si>
+  <si>
+    <t>Lumia 630 / 635</t>
+  </si>
+  <si>
+    <t>Lumia 900</t>
+  </si>
+  <si>
+    <t>Lumia 920</t>
+  </si>
+  <si>
+    <t>Lumia 1320</t>
+  </si>
+  <si>
+    <t>IPHONE</t>
+  </si>
+  <si>
+    <t>SAMSUNG</t>
+  </si>
+  <si>
+    <t>HUAWEI</t>
+  </si>
+  <si>
+    <t>HONOR</t>
+  </si>
+  <si>
+    <t>SONY</t>
+  </si>
+  <si>
+    <t>ONEPLUS</t>
+  </si>
+  <si>
+    <t>XIAOMI</t>
+  </si>
+  <si>
+    <t>ASUS</t>
+  </si>
+  <si>
+    <t>MOTOROLA</t>
+  </si>
+  <si>
+    <t>NOKIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -410,8 +599,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,14 +637,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -480,15 +669,43 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
+      <bottom style="thick">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,13 +713,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -808,1321 +1046,1735 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="20">
         <v>145</v>
       </c>
-      <c r="C2">
+      <c r="D2" s="20">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B3">
+      <c r="C3" s="19">
         <v>139</v>
       </c>
-      <c r="C3">
+      <c r="D3" s="19">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B4">
+      <c r="C4" s="19">
         <v>151</v>
       </c>
-      <c r="C4">
+      <c r="D4" s="19">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B5">
+      <c r="C5" s="19">
         <v>136</v>
       </c>
-      <c r="C5">
+      <c r="D5" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B6">
+      <c r="C6" s="19">
         <v>142</v>
       </c>
-      <c r="C6">
+      <c r="D6" s="19">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B7">
+      <c r="C7" s="19">
         <v>151</v>
       </c>
-      <c r="C7">
+      <c r="D7" s="19">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B8">
+      <c r="C8" s="19">
         <v>115</v>
       </c>
-      <c r="C8">
+      <c r="D8" s="19">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B9">
+      <c r="C9" s="19">
         <v>123</v>
       </c>
-      <c r="C9">
+      <c r="D9" s="19">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B10">
+      <c r="C10" s="19">
         <v>120</v>
       </c>
-      <c r="C10">
+      <c r="D10" s="19">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B11">
+      <c r="C11" s="19">
         <v>132</v>
       </c>
-      <c r="C11">
+      <c r="D11" s="19">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B12">
+      <c r="C12" s="19">
         <v>147</v>
       </c>
-      <c r="C12">
+      <c r="D12" s="19">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B13">
+      <c r="C13" s="19">
         <v>130</v>
       </c>
-      <c r="C13">
+      <c r="D13" s="19">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B14">
+      <c r="C14" s="19">
         <v>151</v>
       </c>
-      <c r="C14">
+      <c r="D14" s="19">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B15">
+      <c r="C15" s="21">
         <v>117</v>
       </c>
-      <c r="C15">
+      <c r="D15" s="21">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="C16" s="20">
         <v>134</v>
       </c>
-      <c r="C16">
+      <c r="D16" s="20">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17">
+      <c r="C17" s="19">
         <v>135</v>
       </c>
-      <c r="C17">
+      <c r="D17" s="19">
         <v>63</v>
       </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B18">
+      <c r="C18" s="19">
         <v>150</v>
       </c>
-      <c r="C18">
+      <c r="D18" s="19">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19">
+      <c r="C19" s="19">
         <v>132</v>
       </c>
-      <c r="C19">
+      <c r="D19" s="19">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B20">
+      <c r="C20" s="19">
         <v>141</v>
       </c>
-      <c r="C20">
+      <c r="D20" s="19">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B21">
+      <c r="C21" s="19">
         <v>140</v>
       </c>
-      <c r="C21">
+      <c r="D21" s="19">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B22">
+      <c r="C22" s="19">
         <v>151</v>
       </c>
-      <c r="C22">
+      <c r="D22" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B23">
+      <c r="C23" s="19">
         <v>140</v>
       </c>
-      <c r="C23">
+      <c r="D23" s="19">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B24">
+      <c r="C24" s="19">
         <v>149</v>
       </c>
-      <c r="C24">
+      <c r="D24" s="19">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B25">
+      <c r="C25" s="19">
         <v>140</v>
       </c>
-      <c r="C25">
+      <c r="D25" s="19">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B26">
+      <c r="C26" s="19">
         <v>130</v>
       </c>
-      <c r="C26">
+      <c r="D26" s="19">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B27">
+      <c r="C27" s="19">
         <v>148</v>
       </c>
-      <c r="C27">
+      <c r="D27" s="19">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B28">
+      <c r="C28" s="19">
         <v>120</v>
       </c>
-      <c r="C28">
+      <c r="D28" s="19">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B29">
+      <c r="C29" s="19">
         <v>130</v>
       </c>
-      <c r="C29">
+      <c r="D29" s="19">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B30">
+      <c r="C30" s="19">
         <v>128</v>
       </c>
-      <c r="C30">
+      <c r="D30" s="19">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B31">
+      <c r="C31" s="19">
         <v>1310</v>
       </c>
-      <c r="C31">
+      <c r="D31" s="19">
         <v>610</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B32">
+      <c r="C32" s="19">
         <v>139</v>
       </c>
-      <c r="C32">
+      <c r="D32" s="19">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B33">
+      <c r="C33" s="19">
         <v>138</v>
       </c>
-      <c r="C33">
+      <c r="D33" s="19">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B34">
+      <c r="C34" s="19">
         <v>138</v>
       </c>
-      <c r="C34">
+      <c r="D34" s="19">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B35">
+      <c r="C35" s="19">
         <v>148</v>
       </c>
-      <c r="C35">
+      <c r="D35" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B36">
+      <c r="C36" s="19">
         <v>141</v>
       </c>
-      <c r="C36">
+      <c r="D36" s="19">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B37">
+      <c r="C37" s="19">
         <v>145</v>
       </c>
-      <c r="C37">
+      <c r="D37" s="19">
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B38">
+      <c r="C38" s="19">
         <v>149</v>
       </c>
-      <c r="C38">
+      <c r="D38" s="19">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B39">
+      <c r="C39" s="19">
         <v>150</v>
       </c>
-      <c r="C39">
+      <c r="D39" s="19">
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B40">
+      <c r="C40" s="19">
         <v>150</v>
       </c>
-      <c r="C40">
+      <c r="D40" s="19">
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B41">
+      <c r="C41" s="19">
         <v>141</v>
       </c>
-      <c r="C41">
+      <c r="D41" s="19">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B42">
+      <c r="C42" s="19">
         <v>151</v>
       </c>
-      <c r="C42">
+      <c r="D42" s="19">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B43">
+      <c r="C43" s="19">
         <v>155</v>
       </c>
-      <c r="C43">
+      <c r="D43" s="19">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B44">
+      <c r="C44" s="19">
         <v>129</v>
       </c>
-      <c r="C44">
+      <c r="D44" s="19">
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B45">
+      <c r="C45" s="19">
         <v>128</v>
       </c>
-      <c r="C45">
+      <c r="D45" s="19">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B46">
+      <c r="C46" s="19">
         <v>136</v>
       </c>
-      <c r="C46">
+      <c r="D46" s="19">
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B47">
+      <c r="C47" s="19">
         <v>129</v>
       </c>
-      <c r="C47">
+      <c r="D47" s="19">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B48">
+      <c r="C48" s="19">
         <v>132</v>
       </c>
-      <c r="C48">
+      <c r="D48" s="19">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B49">
+      <c r="C49" s="19">
         <v>138</v>
       </c>
-      <c r="C49">
+      <c r="D49" s="19">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B50">
+      <c r="C50" s="19">
         <v>137</v>
       </c>
-      <c r="C50">
+      <c r="D50" s="19">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B51">
+      <c r="C51" s="19">
         <v>152</v>
       </c>
-      <c r="C51">
+      <c r="D51" s="19">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B52">
+      <c r="C52" s="19">
         <v>144</v>
       </c>
-      <c r="C52">
+      <c r="D52" s="19">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B53">
+      <c r="C53" s="19">
         <v>148</v>
       </c>
-      <c r="C53">
+      <c r="D53" s="19">
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B54">
+      <c r="C54" s="19">
         <v>146</v>
       </c>
-      <c r="C54">
+      <c r="D54" s="19">
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B55">
+      <c r="C55" s="19">
         <v>150</v>
       </c>
-      <c r="C55">
+      <c r="D55" s="19">
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B56">
+      <c r="C56" s="19">
         <v>154</v>
       </c>
-      <c r="C56">
+      <c r="D56" s="19">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B57">
+      <c r="C57" s="19">
         <v>153</v>
       </c>
-      <c r="C57">
+      <c r="D57" s="19">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B58">
+      <c r="C58" s="19">
         <v>147</v>
       </c>
-      <c r="C58">
+      <c r="D58" s="19">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B59">
+      <c r="C59" s="19">
         <v>157</v>
       </c>
-      <c r="C59">
+      <c r="D59" s="19">
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B60">
+      <c r="C60" s="19">
         <v>134</v>
       </c>
-      <c r="C60">
+      <c r="D60" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B61">
+      <c r="C61" s="19">
         <v>147</v>
       </c>
-      <c r="C61">
+      <c r="D61" s="19">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B62">
+      <c r="C62" s="19">
         <v>147</v>
       </c>
-      <c r="C62">
+      <c r="D62" s="19">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B63">
+      <c r="C63" s="19">
         <v>159</v>
       </c>
-      <c r="C63">
+      <c r="D63" s="19">
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B64">
+      <c r="C64" s="19">
         <v>159</v>
       </c>
-      <c r="C64">
+      <c r="D64" s="19">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B65">
+      <c r="C65" s="19">
         <v>147</v>
       </c>
-      <c r="C65">
+      <c r="D65" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B66">
+      <c r="C66" s="19">
         <v>140</v>
       </c>
-      <c r="C66">
+      <c r="D66" s="19">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B67">
+      <c r="C67" s="19">
         <v>157</v>
       </c>
-      <c r="C67">
+      <c r="D67" s="19">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="12"/>
+      <c r="B68" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B68">
+      <c r="C68" s="21">
         <v>155</v>
       </c>
-      <c r="C68">
+      <c r="D68" s="21">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+    <row r="69" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B69">
+      <c r="C69" s="20">
         <v>139</v>
       </c>
-      <c r="C69">
+      <c r="D69" s="20">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B70">
+      <c r="C70" s="19">
         <v>139</v>
       </c>
-      <c r="C70">
+      <c r="D70" s="19">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B71">
+      <c r="C71" s="19">
         <v>141</v>
       </c>
-      <c r="C71">
+      <c r="D71" s="19">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B72">
+      <c r="C72" s="19">
         <v>134</v>
       </c>
-      <c r="C72">
+      <c r="D72" s="19">
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B73">
+      <c r="C73" s="19">
         <v>139</v>
       </c>
-      <c r="C73">
+      <c r="D73" s="19">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B74">
+      <c r="C74" s="19">
         <v>139</v>
       </c>
-      <c r="C74">
+      <c r="D74" s="19">
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B75">
+      <c r="C75" s="19">
         <v>138</v>
       </c>
-      <c r="C75">
+      <c r="D75" s="19">
         <v>63</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B76">
+      <c r="C76" s="19">
         <v>139</v>
       </c>
-      <c r="C76">
+      <c r="D76" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B77">
+      <c r="C77" s="19">
         <v>140</v>
       </c>
-      <c r="C77">
+      <c r="D77" s="19">
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B78">
+      <c r="C78" s="19">
         <v>148</v>
       </c>
-      <c r="C78">
+      <c r="D78" s="19">
         <v>66</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B79">
+      <c r="C79" s="19">
         <v>142</v>
       </c>
-      <c r="C79">
+      <c r="D79" s="19">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B80">
+      <c r="C80" s="19">
         <v>139</v>
       </c>
-      <c r="C80">
+      <c r="D80" s="19">
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B81">
+      <c r="C81" s="19">
         <v>144</v>
       </c>
-      <c r="C81">
+      <c r="D81" s="19">
         <v>63</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B82">
+      <c r="C82" s="19">
         <v>142</v>
       </c>
-      <c r="C82">
+      <c r="D82" s="19">
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B83">
+      <c r="C83" s="19">
         <v>139</v>
       </c>
-      <c r="C83">
+      <c r="D83" s="19">
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B84">
+      <c r="C84" s="19">
         <v>149</v>
       </c>
-      <c r="C84">
+      <c r="D84" s="19">
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B85">
+      <c r="C85" s="19">
         <v>150</v>
       </c>
-      <c r="C85">
+      <c r="D85" s="19">
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B86">
+      <c r="C86" s="19">
         <v>140</v>
       </c>
-      <c r="C86">
+      <c r="D86" s="19">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B87">
+      <c r="C87" s="19">
         <v>146</v>
       </c>
-      <c r="C87">
+      <c r="D87" s="19">
         <v>66</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B88">
+      <c r="C88" s="19">
         <v>148</v>
       </c>
-      <c r="C88">
+      <c r="D88" s="19">
         <v>67</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B89">
+      <c r="C89" s="19">
         <v>151</v>
       </c>
-      <c r="C89">
+      <c r="D89" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B90">
+      <c r="C90" s="19">
         <v>148</v>
       </c>
-      <c r="C90">
+      <c r="D90" s="19">
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="12"/>
+      <c r="B91" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B91">
+      <c r="C91" s="21">
         <v>150</v>
       </c>
-      <c r="C91">
+      <c r="D91" s="21">
         <v>67</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+    <row r="92" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B92" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B92">
+      <c r="C92" s="20">
         <v>135</v>
       </c>
-      <c r="C92">
+      <c r="D92" s="20">
         <v>66</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B93">
+      <c r="C93" s="19">
         <v>135</v>
       </c>
-      <c r="C93">
+      <c r="D93" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B94">
+      <c r="C94" s="19">
         <v>138</v>
       </c>
-      <c r="C94">
+      <c r="D94" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B95">
+      <c r="C95" s="19">
         <v>152</v>
       </c>
-      <c r="C95">
+      <c r="D95" s="19">
         <v>66</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B96">
+      <c r="C96" s="19">
         <v>138</v>
       </c>
-      <c r="C96">
+      <c r="D96" s="19">
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B97">
+      <c r="C97" s="19">
         <v>140</v>
       </c>
-      <c r="C97">
+      <c r="D97" s="19">
         <v>61</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B98">
+      <c r="C98" s="19">
         <v>150</v>
       </c>
-      <c r="C98">
+      <c r="D98" s="19">
         <v>63</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B99">
+      <c r="C99" s="19">
         <v>140</v>
       </c>
-      <c r="C99">
+      <c r="D99" s="19">
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B100">
+      <c r="C100" s="19">
         <v>141</v>
       </c>
-      <c r="C100">
+      <c r="D100" s="19">
         <v>62</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B101">
+      <c r="C101" s="19">
         <v>153</v>
       </c>
-      <c r="C101">
+      <c r="D101" s="19">
         <v>70</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="12"/>
+      <c r="B102" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B102">
+      <c r="C102" s="21">
         <v>155</v>
       </c>
-      <c r="C102">
+      <c r="D102" s="21">
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
+    <row r="103" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B103">
+      <c r="C103" s="20">
         <v>145</v>
       </c>
-      <c r="C103">
+      <c r="D103" s="20">
         <v>64</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B104">
+      <c r="C104" s="19">
         <v>145</v>
       </c>
-      <c r="C104">
+      <c r="D104" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B105">
+      <c r="C105" s="19">
         <v>145</v>
       </c>
-      <c r="C105">
+      <c r="D105" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B106">
+      <c r="C106" s="19">
         <v>142</v>
       </c>
-      <c r="C106">
+      <c r="D106" s="19">
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B107">
+      <c r="C107" s="19">
         <v>123</v>
       </c>
-      <c r="C107">
+      <c r="D107" s="19">
         <v>60</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B108">
+      <c r="C108" s="19">
         <v>160</v>
       </c>
-      <c r="C108">
+      <c r="D108" s="19">
         <v>80</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B109">
+      <c r="C109" s="19">
         <v>138</v>
       </c>
-      <c r="C109">
+      <c r="D109" s="19">
         <v>64</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B110">
+      <c r="C110" s="19">
         <v>138</v>
       </c>
-      <c r="C110">
+      <c r="D110" s="19">
         <v>65</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B111">
+      <c r="C111" s="19">
         <v>160</v>
       </c>
-      <c r="C111">
+      <c r="D111" s="19">
         <v>71</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B112">
+      <c r="C112" s="19">
         <v>141</v>
       </c>
-      <c r="C112">
+      <c r="D112" s="19">
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B113">
+      <c r="C113" s="19">
         <v>160</v>
       </c>
-      <c r="C113">
+      <c r="D113" s="19">
         <v>70</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B114">
+      <c r="C114" s="19">
         <v>160</v>
       </c>
-      <c r="C114">
+      <c r="D114" s="19">
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B115">
+      <c r="C115" s="19">
         <v>143</v>
       </c>
-      <c r="C115">
+      <c r="D115" s="19">
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B116">
+      <c r="C116" s="19">
         <v>145</v>
       </c>
-      <c r="C116">
+      <c r="D116" s="19">
         <v>67</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B117">
+      <c r="C117" s="19">
         <v>133</v>
       </c>
-      <c r="C117">
+      <c r="D117" s="19">
         <v>56</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
+    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="12"/>
+      <c r="B118" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B118">
+      <c r="C118" s="21">
         <v>141</v>
       </c>
-      <c r="C118">
+      <c r="D118" s="21">
         <v>55</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="4"/>
+    <row r="119" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B119" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C119" s="20"/>
+      <c r="D119" s="20"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C120" s="19"/>
+      <c r="D120" s="19"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C121" s="19"/>
+      <c r="D121" s="19"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C123" s="19"/>
+      <c r="D123" s="19"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
+    </row>
+    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="12"/>
+      <c r="B125" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C125" s="21"/>
+      <c r="D125" s="21"/>
+    </row>
+    <row r="126" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B126" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C126" s="20"/>
+      <c r="D126" s="20"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C127" s="19"/>
+      <c r="D127" s="19"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C128" s="19"/>
+      <c r="D128" s="19"/>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C130" s="19"/>
+      <c r="D130" s="19"/>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C131" s="19"/>
+      <c r="D131" s="19"/>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C132" s="19"/>
+      <c r="D132" s="19"/>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C133" s="19"/>
+      <c r="D133" s="19"/>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C134" s="19"/>
+      <c r="D134" s="19"/>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C135" s="19"/>
+      <c r="D135" s="19"/>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C136" s="19"/>
+      <c r="D136" s="19"/>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C137" s="19"/>
+      <c r="D137" s="19"/>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C138" s="19"/>
+      <c r="D138" s="19"/>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C139" s="19"/>
+      <c r="D139" s="19"/>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C140" s="19"/>
+      <c r="D140" s="19"/>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C141" s="19"/>
+      <c r="D141" s="19"/>
+    </row>
+    <row r="142" spans="2:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B142" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C142" s="19"/>
+      <c r="D142" s="19"/>
+    </row>
+    <row r="143" spans="2:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B143" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C143" s="19"/>
+      <c r="D143" s="19"/>
+    </row>
+    <row r="144" spans="2:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B144" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C144" s="19"/>
+      <c r="D144" s="19"/>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="12"/>
+      <c r="B145" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C145" s="21"/>
+      <c r="D145" s="21"/>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B146" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C146" s="20"/>
+      <c r="D146" s="20"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C147" s="19"/>
+      <c r="D147" s="19"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C148" s="19"/>
+      <c r="D148" s="19"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C149" s="19"/>
+      <c r="D149" s="19"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C150" s="19"/>
+      <c r="D150" s="19"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C151" s="19"/>
+      <c r="D151" s="19"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C152" s="19"/>
+      <c r="D152" s="19"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C153" s="19"/>
+      <c r="D153" s="19"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C154" s="19"/>
+      <c r="D154" s="19"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C155" s="19"/>
+      <c r="D155" s="19"/>
+    </row>
+    <row r="156" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="12"/>
+      <c r="B156" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C156" s="21"/>
+      <c r="D156" s="21"/>
+    </row>
+    <row r="157" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B157" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C157" s="20"/>
+      <c r="D157" s="20"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C158" s="19"/>
+      <c r="D158" s="19"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C159" s="19"/>
+      <c r="D159" s="19"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C160" s="19"/>
+      <c r="D160" s="19"/>
+    </row>
+    <row r="161" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="12"/>
+      <c r="B161" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C161" s="21"/>
+      <c r="D161" s="21"/>
+    </row>
+    <row r="162" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B162" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C162" s="20"/>
+      <c r="D162" s="20"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C163" s="19"/>
+      <c r="D163" s="19"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C164" s="19"/>
+      <c r="D164" s="19"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C165" s="19"/>
+      <c r="D165" s="19"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C166" s="19"/>
+      <c r="D166" s="19"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C167" s="19"/>
+      <c r="D167" s="19"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C168" s="19"/>
+      <c r="D168" s="19"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C169" s="19"/>
+      <c r="D169" s="19"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C170" s="19"/>
+      <c r="D170" s="19"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C171" s="19"/>
+      <c r="D171" s="19"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C172" s="19"/>
+      <c r="D172" s="19"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
Ajout Redimensionnement des POP
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetDDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30F2871-3AB4-456D-8F66-0B663C7D62FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAA69F7-6EFB-472B-BF99-B53EC653DB3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26100" yWindow="-705" windowWidth="18000" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-2850" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
   <si>
     <t>Modèle</t>
   </si>
@@ -551,6 +551,12 @@
   </si>
   <si>
     <t>GALAXYNOTE10</t>
+  </si>
+  <si>
+    <t>GALAXYJ6+2018</t>
+  </si>
+  <si>
+    <t>POP</t>
   </si>
 </sst>
 </file>
@@ -1037,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H166"/>
+  <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,55 +1080,55 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C4" s="5">
         <v>145</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D4" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="5">
         <v>139</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D5" s="5">
         <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5">
-        <v>151</v>
-      </c>
-      <c r="D5" s="5">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="5">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="D6" s="5">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5">
         <v>136</v>
@@ -1133,51 +1139,51 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="C8" s="5">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D8" s="5">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D9" s="5">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="D10" s="5">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D11" s="5">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>123</v>
@@ -1188,29 +1194,29 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D13" s="5">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D14" s="5">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="C15" s="5">
         <v>132</v>
@@ -1221,18 +1227,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="C16" s="5">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="D16" s="5">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="C17" s="5">
         <v>147</v>
@@ -1243,18 +1249,18 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="D18" s="5">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="5">
         <v>130</v>
@@ -1265,18 +1271,18 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="5">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="D20" s="5">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="5">
         <v>151</v>
@@ -1286,30 +1292,30 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="5">
+        <v>151</v>
+      </c>
+      <c r="D22" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C23" s="5">
         <v>107</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D23" s="5">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="C23" s="5">
-        <v>117</v>
-      </c>
-      <c r="D23" s="5">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="C24" s="5">
         <v>117</v>
@@ -1319,286 +1325,286 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="B25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="5">
+        <v>117</v>
+      </c>
+      <c r="D25" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C26" s="7">
         <v>134</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D26" s="7">
         <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="7">
-        <v>135</v>
-      </c>
-      <c r="D26" s="7">
-        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="7">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D27" s="7">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="7">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D28" s="7">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="7">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D29" s="7">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="7">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D30" s="7">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" s="7">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D31" s="7">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="7">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D32" s="7">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="7">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D33" s="7">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="7">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="D34" s="7">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="7">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D35" s="7">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="7">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="D36" s="7">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="7">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="D37" s="7">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" s="7">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D38" s="7">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" s="7">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D39" s="7">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="7">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D40" s="7">
-        <v>610</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="7">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D41" s="7">
-        <v>66</v>
+        <v>610</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="7">
+        <v>139</v>
+      </c>
+      <c r="D42" s="7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C43" s="7">
         <v>138</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D43" s="7">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C44" s="7">
         <v>152</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D44" s="7">
         <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="7">
-        <v>138</v>
-      </c>
-      <c r="D44" s="7">
-        <v>59</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" s="7">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D45" s="7">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" s="7">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="D46" s="7">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" s="7">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D47" s="7">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="7">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D48" s="7">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" s="7">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D49" s="7">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C50" s="7">
         <v>150</v>
@@ -1609,73 +1615,73 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" s="7">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="D51" s="7">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" s="7">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D52" s="7">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" s="7">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D53" s="7">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C54" s="7">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D54" s="7">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="7">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D55" s="7">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="7">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D56" s="7">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="7">
         <v>159</v>
@@ -1686,73 +1692,73 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="7">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="D58" s="7">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="7">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D59" s="7">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="7">
+        <v>140</v>
+      </c>
+      <c r="D60" s="7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C61" s="7">
         <v>157</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D61" s="7">
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="7" t="s">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C62" s="7">
         <v>162</v>
       </c>
-      <c r="D61" s="7">
+      <c r="D62" s="7">
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="6" t="s">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C63" s="7">
         <v>155</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D63" s="7">
         <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C63" s="7">
-        <v>143</v>
-      </c>
-      <c r="D63" s="7">
-        <v>73</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C64" s="7">
         <v>143</v>
@@ -1762,19 +1768,19 @@
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="6" t="s">
-        <v>50</v>
+      <c r="B65" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="C65" s="7">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="D65" s="7">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="C66" s="7">
         <v>129</v>
@@ -1785,73 +1791,73 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
       <c r="C67" s="7">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D67" s="7">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" s="7">
+        <v>128</v>
+      </c>
+      <c r="D68" s="7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C69" s="7">
         <v>136</v>
       </c>
-      <c r="D68" s="7">
+      <c r="D69" s="7">
         <v>62</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C69" s="7">
-        <v>143</v>
-      </c>
-      <c r="D69" s="7">
-        <v>70</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="7">
+        <v>143</v>
+      </c>
+      <c r="D70" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C71" s="7">
         <v>151</v>
       </c>
-      <c r="D70" s="7">
+      <c r="D71" s="7">
         <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C71" s="7">
-        <v>163</v>
-      </c>
-      <c r="D71" s="7">
-        <v>79</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="6" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C72" s="7">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="D72" s="7">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="6" t="s">
-        <v>138</v>
+        <v>53</v>
       </c>
       <c r="C73" s="7">
         <v>129</v>
@@ -1862,54 +1868,54 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="6" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="C74" s="7">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D74" s="7">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C75" s="7">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D75" s="7">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C76" s="7">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D76" s="7">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C77" s="7">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D77" s="7">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C78" s="7">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="D78" s="7">
         <v>70</v>
@@ -1917,10 +1923,10 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="6" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="C79" s="7">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="D79" s="7">
         <v>70</v>
@@ -1928,255 +1934,255 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C80" s="7">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D80" s="7">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" s="6" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C81" s="7">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D81" s="7">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C82" s="7">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D82" s="7">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C83" s="7">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D83" s="7">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" s="7">
+        <v>150</v>
+      </c>
+      <c r="D84" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" s="7">
+        <v>154</v>
+      </c>
+      <c r="D85" s="7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C86" s="7">
         <v>153</v>
       </c>
-      <c r="D84" s="7">
+      <c r="D86" s="7">
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="6" t="s">
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C87" s="7">
         <v>147</v>
       </c>
-      <c r="D85" s="7">
+      <c r="D87" s="7">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="6" t="s">
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C88" s="7">
         <v>157</v>
       </c>
-      <c r="D86" s="7">
+      <c r="D88" s="7">
         <v>73</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="7" t="s">
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C89" s="7">
         <v>169</v>
       </c>
-      <c r="D87" s="7">
+      <c r="D89" s="7">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="6" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C88" s="7">
+      <c r="C90" s="7">
         <v>134</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D90" s="7">
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B91" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C91" s="9">
         <v>139</v>
       </c>
-      <c r="D89" s="9">
+      <c r="D91" s="9">
         <v>66</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C90" s="9">
-        <v>139</v>
-      </c>
-      <c r="D90" s="9">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C91" s="9">
-        <v>141</v>
-      </c>
-      <c r="D91" s="9">
-        <v>67</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C92" s="9">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D92" s="9">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C93" s="9">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D93" s="9">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C94" s="9">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D94" s="9">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B95" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C95" s="9">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D95" s="9">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B96" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C96" s="9">
         <v>139</v>
       </c>
       <c r="D96" s="9">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C97" s="9">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D97" s="9">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C98" s="9">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D98" s="9">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C99" s="9">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D99" s="9">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C100" s="9">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="D100" s="9">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C101" s="9">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D101" s="9">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C102" s="9">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D102" s="9">
         <v>63</v>
@@ -2184,21 +2190,21 @@
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="8" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C103" s="9">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D103" s="9">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="8" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C104" s="9">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D104" s="9">
         <v>63</v>
@@ -2206,694 +2212,694 @@
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C105" s="9">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="D105" s="9">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="8" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C106" s="9">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D106" s="9">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="8" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="C107" s="9">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="D107" s="9">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C108" s="9">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D108" s="9">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C109" s="9">
+        <v>140</v>
+      </c>
+      <c r="D109" s="9">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C110" s="9">
+        <v>146</v>
+      </c>
+      <c r="D110" s="9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="C109" s="9">
-        <v>148</v>
-      </c>
-      <c r="D109" s="9">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C110" s="9">
-        <v>151</v>
-      </c>
-      <c r="D110" s="9">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="C111" s="9">
         <v>148</v>
       </c>
       <c r="D111" s="9">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C112" s="9">
+        <v>151</v>
+      </c>
+      <c r="D112" s="9">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C113" s="9">
+        <v>148</v>
+      </c>
+      <c r="D113" s="9">
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="8" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B114" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C112" s="9">
+      <c r="C114" s="9">
         <v>150</v>
       </c>
-      <c r="D112" s="9">
+      <c r="D114" s="9">
         <v>67</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B113" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C113" s="9">
-        <v>142</v>
-      </c>
-      <c r="D113" s="9">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B114" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C114" s="9">
-        <v>142</v>
-      </c>
-      <c r="D114" s="9">
-        <v>71</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B115" s="9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C115" s="9">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D115" s="9">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B116" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C116" s="9">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D116" s="9">
         <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B117" s="8" t="s">
-        <v>94</v>
+      <c r="B117" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="C117" s="9">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D117" s="9">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B118" s="8" t="s">
-        <v>95</v>
+      <c r="B118" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="C118" s="9">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D118" s="9">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B119" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C119" s="9">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="D119" s="9">
-        <v>81</v>
-      </c>
-      <c r="F119" t="s">
-        <v>98</v>
-      </c>
-      <c r="G119">
-        <v>164</v>
-      </c>
-      <c r="H119">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B120" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C120" s="9">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="D120" s="9">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B121" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C121" s="9">
+        <v>164</v>
+      </c>
+      <c r="D121" s="9">
+        <v>81</v>
+      </c>
+      <c r="F121" t="s">
+        <v>98</v>
+      </c>
+      <c r="G121">
+        <v>164</v>
+      </c>
+      <c r="H121">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B122" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C122" s="9">
+        <v>163</v>
+      </c>
+      <c r="D122" s="9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B123" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C121" s="9">
+      <c r="C123" s="9">
         <v>159</v>
       </c>
-      <c r="D121" s="9">
+      <c r="D123" s="9">
         <v>78</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="11" t="s">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B122" s="11" t="s">
+      <c r="B124" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C122" s="11">
+      <c r="C124" s="11">
         <v>153</v>
       </c>
-      <c r="D122" s="11">
+      <c r="D124" s="11">
         <v>79</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B123" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C123" s="11">
-        <v>151</v>
-      </c>
-      <c r="D123" s="11">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B124" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C124" s="11">
-        <v>135</v>
-      </c>
-      <c r="D124" s="11">
-        <v>66</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B125" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C125" s="11">
+        <v>151</v>
+      </c>
+      <c r="D125" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C126" s="11">
+        <v>135</v>
+      </c>
+      <c r="D126" s="11">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C125" s="11">
+      <c r="C127" s="11">
         <v>152</v>
       </c>
-      <c r="D125" s="11">
+      <c r="D127" s="11">
         <v>73</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="11" t="s">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B128" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C126" s="11">
+      <c r="C128" s="11">
         <v>150</v>
       </c>
-      <c r="D126" s="11">
+      <c r="D128" s="11">
         <v>72</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B127" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C127" s="11">
-        <v>135</v>
-      </c>
-      <c r="D127" s="11">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B128" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C128" s="11">
-        <v>138</v>
-      </c>
-      <c r="D128" s="11">
-        <v>64</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C129" s="11">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D129" s="11">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C130" s="11">
         <v>138</v>
       </c>
       <c r="D130" s="11">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="11" t="s">
-        <v>129</v>
+      <c r="B131" s="10" t="s">
+        <v>150</v>
       </c>
       <c r="C131" s="11">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D131" s="11">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C132" s="11">
+        <v>138</v>
+      </c>
+      <c r="D132" s="11">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C133" s="11">
+        <v>139</v>
+      </c>
+      <c r="D133" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C132" s="11">
+      <c r="C134" s="11">
         <v>140</v>
       </c>
-      <c r="D132" s="11">
+      <c r="D134" s="11">
         <v>61</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C133" s="11">
-        <v>150</v>
-      </c>
-      <c r="D133" s="11">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C134" s="11">
-        <v>159</v>
-      </c>
-      <c r="D134" s="11">
-        <v>77</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C135" s="11">
+        <v>150</v>
+      </c>
+      <c r="D135" s="11">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C136" s="11">
+        <v>159</v>
+      </c>
+      <c r="D136" s="11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C135" s="11">
+      <c r="C137" s="11">
         <v>155</v>
       </c>
-      <c r="D135" s="11">
+      <c r="D137" s="11">
         <v>74</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="13" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B136" s="12" t="s">
+      <c r="B138" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="C136" s="13">
+      <c r="C138" s="13">
         <v>145</v>
       </c>
-      <c r="D136" s="13">
+      <c r="D138" s="13">
         <v>64</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C137" s="13">
-        <v>156</v>
-      </c>
-      <c r="D137" s="13">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C138" s="13">
-        <v>152</v>
-      </c>
-      <c r="D138" s="13">
-        <v>70</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B139" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C139" s="13">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="D139" s="13">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="13" t="s">
-        <v>159</v>
+      <c r="B140" s="12" t="s">
+        <v>157</v>
       </c>
       <c r="C140" s="13">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D140" s="13">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B141" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C141" s="13">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D141" s="13">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="12" t="s">
-        <v>161</v>
+      <c r="B142" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="C142" s="13">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D142" s="13">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C143" s="13">
         <v>138</v>
       </c>
       <c r="D143" s="13">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C144" s="13">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="D144" s="13">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C145" s="13">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D145" s="13">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C146" s="13">
         <v>160</v>
       </c>
       <c r="D146" s="13">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C147" s="13">
+        <v>141</v>
+      </c>
+      <c r="D147" s="13">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C148" s="13">
         <v>160</v>
       </c>
-      <c r="D147" s="13">
+      <c r="D148" s="13">
         <v>70</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="C148" s="13">
-        <v>168</v>
-      </c>
-      <c r="D148" s="13">
-        <v>82</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C149" s="13">
+        <v>160</v>
+      </c>
+      <c r="D149" s="13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C150" s="13">
         <v>168</v>
       </c>
-      <c r="C149" s="13">
-        <v>143</v>
-      </c>
-      <c r="D149" s="13">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C150" s="13">
-        <v>145</v>
-      </c>
       <c r="D150" s="13">
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C151" s="13">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D151" s="13">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C152" s="13">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D152" s="13">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C153" s="13">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D153" s="13">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C154" s="13">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="D154" s="13">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B155" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C155" s="13">
+        <v>142</v>
+      </c>
+      <c r="D155" s="13">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C156" s="13">
+        <v>123</v>
+      </c>
+      <c r="D156" s="13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="C155" s="13">
+      <c r="C157" s="13">
         <v>160</v>
       </c>
-      <c r="D155" s="13">
+      <c r="D157" s="13">
         <v>80</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="14" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="B156" s="14" t="s">
+      <c r="B158" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="C156" s="14">
+      <c r="C158" s="14">
         <v>159</v>
       </c>
-      <c r="D156" s="14">
+      <c r="D158" s="14">
         <v>76</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C157" s="14">
-        <v>159</v>
-      </c>
-      <c r="D157" s="14">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C158" s="14">
-        <v>150</v>
-      </c>
-      <c r="D158" s="14">
-        <v>74</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C159" s="14">
+        <v>159</v>
+      </c>
+      <c r="D159" s="14">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C160" s="14">
+        <v>150</v>
+      </c>
+      <c r="D160" s="14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C159" s="14">
+      <c r="C161" s="14">
         <v>150</v>
       </c>
-      <c r="D159" s="14">
+      <c r="D161" s="14">
         <v>75</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="15" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B160" s="15" t="s">
+      <c r="B162" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C160" s="15">
+      <c r="C162" s="15">
         <v>152</v>
       </c>
-      <c r="D160" s="15">
+      <c r="D162" s="15">
         <v>75</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="15" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C161" s="15">
+      <c r="C163" s="15">
         <v>147</v>
       </c>
-      <c r="D161" s="15">
+      <c r="D163" s="15">
         <v>75</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="16" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="B162" s="16" t="s">
+      <c r="B164" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C162" s="16">
+      <c r="C164" s="16">
         <v>160</v>
       </c>
-      <c r="D162" s="16">
+      <c r="D164" s="16">
         <v>80</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="17" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="B163" s="17" t="s">
+      <c r="B165" s="17" t="s">
         <v>127</v>
-      </c>
-      <c r="C163" s="17">
-        <v>155</v>
-      </c>
-      <c r="D163" s="17">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C164" s="17">
-        <v>157</v>
-      </c>
-      <c r="D164" s="17">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="17" t="s">
-        <v>118</v>
       </c>
       <c r="C165" s="17">
         <v>155</v>
@@ -2904,12 +2910,34 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B166" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C166" s="17">
+        <v>157</v>
+      </c>
+      <c r="D166" s="17">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C167" s="17">
+        <v>155</v>
+      </c>
+      <c r="D167" s="17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C166" s="17">
+      <c r="C168" s="17">
         <v>159</v>
       </c>
-      <c r="D166" s="17">
+      <c r="D168" s="17">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trie des pages par numéro de commandes
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetDDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808E20AB-2BB5-4BDC-A0D9-4BC52372C3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4B21F8-0924-466F-8282-DB32D7013FFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2805" windowWidth="18000" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5310" yWindow="1845" windowWidth="18000" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout fonctionnalitées + css
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetDDC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D217B62-AEA9-4BCB-94BA-86F21DEE1A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23985" windowHeight="10410"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -109,301 +103,301 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>GALAXYS6</t>
-  </si>
-  <si>
-    <t>GALAXYS6EDGE</t>
-  </si>
-  <si>
-    <t>GALAXYS6EDGE+</t>
-  </si>
-  <si>
-    <t>GALAXYS7</t>
-  </si>
-  <si>
-    <t>GALAXYS7EDGE</t>
-  </si>
-  <si>
-    <t>GALAXYS8</t>
-  </si>
-  <si>
-    <t>GALAXYS8+</t>
-  </si>
-  <si>
-    <t>GALAXYS9</t>
-  </si>
-  <si>
-    <t>GALAXYS9+</t>
-  </si>
-  <si>
-    <t>GALAXYS10</t>
-  </si>
-  <si>
-    <t>GALAXYS10E</t>
-  </si>
-  <si>
-    <t>GALAXYS10+</t>
-  </si>
-  <si>
-    <t>GALAXYA3</t>
-  </si>
-  <si>
-    <t>GALAXYA32016</t>
-  </si>
-  <si>
-    <t>GALAXYA32017</t>
-  </si>
-  <si>
-    <t>GALAXYA5</t>
-  </si>
-  <si>
-    <t>GALAXYA52016</t>
-  </si>
-  <si>
-    <t>GALAXYA52017</t>
-  </si>
-  <si>
-    <t>GALAXYA52018</t>
-  </si>
-  <si>
-    <t>GALAXYA62018</t>
-  </si>
-  <si>
-    <t>GALAXYA6+2018</t>
-  </si>
-  <si>
-    <t>GALAXYA7</t>
-  </si>
-  <si>
-    <t>GALAXYA72016</t>
-  </si>
-  <si>
-    <t>GALAXYA72017</t>
-  </si>
-  <si>
-    <t>GALAXYA72018</t>
-  </si>
-  <si>
-    <t>GALAXYA8</t>
-  </si>
-  <si>
-    <t>GALAXYA82018</t>
-  </si>
-  <si>
-    <t>GALAXYA8+2018</t>
-  </si>
-  <si>
-    <t>GALAXYA9</t>
-  </si>
-  <si>
-    <t>GALAXYA10</t>
-  </si>
-  <si>
-    <t>GALAXYA10E</t>
-  </si>
-  <si>
-    <t>GALAXYA20</t>
-  </si>
-  <si>
-    <t>GALAXYA30</t>
-  </si>
-  <si>
-    <t>GALAXYA20E</t>
-  </si>
-  <si>
-    <t>GALAXYA40</t>
-  </si>
-  <si>
-    <t>GALAXYA50</t>
-  </si>
-  <si>
-    <t>GALAXYA60</t>
-  </si>
-  <si>
-    <t>GALAXYA70</t>
-  </si>
-  <si>
-    <t>GALAXYJ22018</t>
-  </si>
-  <si>
-    <t>GALAXYJ2PRO2018</t>
-  </si>
-  <si>
-    <t>GALAXYJ3</t>
-  </si>
-  <si>
-    <t>GALAXYJ32015</t>
-  </si>
-  <si>
-    <t>GALAXYJ32016</t>
-  </si>
-  <si>
-    <t>GALAXYJ32017</t>
-  </si>
-  <si>
-    <t>GALAXYJ32018</t>
-  </si>
-  <si>
-    <t>GALAXYJ42018</t>
-  </si>
-  <si>
-    <t>GALAXYJ4+2018</t>
-  </si>
-  <si>
-    <t>GALAXYJ5</t>
-  </si>
-  <si>
-    <t>GALAXYJ52015</t>
-  </si>
-  <si>
-    <t>GALAXYJ52016</t>
-  </si>
-  <si>
-    <t>GALAXYJ52017</t>
-  </si>
-  <si>
-    <t>GALAXYJ6</t>
-  </si>
-  <si>
-    <t>GALAXYJ6+</t>
-  </si>
-  <si>
-    <t>GALAXYJ6+2018</t>
-  </si>
-  <si>
-    <t>GALAXYJ7</t>
-  </si>
-  <si>
-    <t>GALAXYJ72015</t>
-  </si>
-  <si>
-    <t>GALAXYJ72016</t>
-  </si>
-  <si>
-    <t>GALAXYJ72017</t>
-  </si>
-  <si>
-    <t>GALAXYJ82018</t>
-  </si>
-  <si>
-    <t>GALAXYNOTE8</t>
-  </si>
-  <si>
-    <t>GALAXYNOTE9</t>
-  </si>
-  <si>
-    <t>GALAXYNOTE10</t>
-  </si>
-  <si>
-    <t>GALAXYNOTE10+</t>
-  </si>
-  <si>
-    <t>GALAXYNOTE10PRO</t>
-  </si>
-  <si>
-    <t>GALAXYGRANDPRIME</t>
+    <t>SAMSUNGGALAXYS6</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS6EDGE</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS6EDGE+</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS7</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS7EDGE</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS8</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS8+</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS9</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS9+</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS10</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS10E</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYS10+</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA3</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA32016</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA32017</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA5</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA52016</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA52017</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA52018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA62018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA6+2018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA7</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA72016</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA72017</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA72018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA8</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA82018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA8+2018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA9</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA10</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA10E</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA20</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA30</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA20E</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA40</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA50</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA60</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYA70</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ22018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ2PRO2018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ3</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ32015</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ32016</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ32017</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ32018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ42018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ4+2018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ5</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ52015</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ52016</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ52017</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ6</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ6+</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ6+2018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ7</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ72015</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ72016</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ72017</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYJ82018</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYNOTE8</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYNOTE9</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYNOTE10</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYNOTE10+</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYNOTE10PRO</t>
+  </si>
+  <si>
+    <t>SAMSUNGGALAXYGRANDPRIME</t>
   </si>
   <si>
     <t>HUAWEI</t>
   </si>
   <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>P8LITE</t>
-  </si>
-  <si>
-    <t>P8LITE2017</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>P9LITE</t>
-  </si>
-  <si>
-    <t>P9+</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P10LITE</t>
-  </si>
-  <si>
-    <t>P20</t>
-  </si>
-  <si>
-    <t>P20PRO</t>
-  </si>
-  <si>
-    <t>P20LITE</t>
-  </si>
-  <si>
-    <t>P30</t>
-  </si>
-  <si>
-    <t>P30PRO</t>
-  </si>
-  <si>
-    <t>P30LITE</t>
-  </si>
-  <si>
-    <t>PSMART</t>
-  </si>
-  <si>
-    <t>PSMART2019</t>
-  </si>
-  <si>
-    <t>MATE8</t>
-  </si>
-  <si>
-    <t>MATE9</t>
-  </si>
-  <si>
-    <t>MATE10</t>
-  </si>
-  <si>
-    <t>MATE10PRO</t>
-  </si>
-  <si>
-    <t>MATE10LITE</t>
-  </si>
-  <si>
-    <t>MATE20</t>
-  </si>
-  <si>
-    <t>MATE20PRO</t>
-  </si>
-  <si>
-    <t>MATE20LITE</t>
-  </si>
-  <si>
-    <t>ENJOY6S</t>
-  </si>
-  <si>
-    <t>Y32017</t>
-  </si>
-  <si>
-    <t>Y52017</t>
-  </si>
-  <si>
-    <t>Y52018</t>
-  </si>
-  <si>
-    <t>Y52019</t>
-  </si>
-  <si>
-    <t>Y62018</t>
-  </si>
-  <si>
-    <t>Y62019</t>
-  </si>
-  <si>
-    <t>Y72019</t>
-  </si>
-  <si>
-    <t>Y72018</t>
+    <t>HUAWEIP8</t>
+  </si>
+  <si>
+    <t>HUAWEIP8LITE</t>
+  </si>
+  <si>
+    <t>HUAWEIP8LITE2017</t>
+  </si>
+  <si>
+    <t>HUAWEIP9</t>
+  </si>
+  <si>
+    <t>HUAWEIP9LITE</t>
+  </si>
+  <si>
+    <t>HUAWEIP9+</t>
+  </si>
+  <si>
+    <t>HUAWEIP10</t>
+  </si>
+  <si>
+    <t>HUAWEIP10LITE</t>
+  </si>
+  <si>
+    <t>HUAWEIP20</t>
+  </si>
+  <si>
+    <t>HUAWEIP20PRO</t>
+  </si>
+  <si>
+    <t>HUAWEIP20LITE</t>
+  </si>
+  <si>
+    <t>HUAWEIP30</t>
+  </si>
+  <si>
+    <t>HUAWEIP30PRO</t>
+  </si>
+  <si>
+    <t>HUAWEIP30LITE</t>
+  </si>
+  <si>
+    <t>HUAWEIPSMART</t>
+  </si>
+  <si>
+    <t>HUAWEIPSMART2019</t>
+  </si>
+  <si>
+    <t>HUAWEIMATE8</t>
+  </si>
+  <si>
+    <t>HUAWEIMATE9</t>
+  </si>
+  <si>
+    <t>HUAWEIMATE10</t>
+  </si>
+  <si>
+    <t>HUAWEIMATE10PRO</t>
+  </si>
+  <si>
+    <t>HUAWEIMATE10LITE</t>
+  </si>
+  <si>
+    <t>HUAWEIMATE20</t>
+  </si>
+  <si>
+    <t>HUAWEIMATE20PRO</t>
+  </si>
+  <si>
+    <t>HUAWEIMATE20LITE</t>
+  </si>
+  <si>
+    <t>HUAWEIENJOHUAWEIY6S</t>
+  </si>
+  <si>
+    <t>HUAWEIY32017</t>
+  </si>
+  <si>
+    <t>HUAWEIY52017</t>
+  </si>
+  <si>
+    <t>HUAWEIY52018</t>
+  </si>
+  <si>
+    <t>HUAWEIY52019</t>
+  </si>
+  <si>
+    <t>HUAWEIY62018</t>
+  </si>
+  <si>
+    <t>HUAWEIY62019</t>
+  </si>
+  <si>
+    <t>HUAWEIY72019</t>
+  </si>
+  <si>
+    <t>HUAWEIY72018</t>
   </si>
   <si>
     <t>Honor</t>
@@ -520,16 +514,16 @@
     <t>XIAOMI</t>
   </si>
   <si>
-    <t>REDMINOTE5</t>
-  </si>
-  <si>
-    <t>REDMI5+</t>
-  </si>
-  <si>
-    <t>REDMI6</t>
-  </si>
-  <si>
-    <t>REDMI6A</t>
+    <t>XIAOMIREDMINOTE5</t>
+  </si>
+  <si>
+    <t>XIAOMIREDMI5+</t>
+  </si>
+  <si>
+    <t>XIAOMIREDMI6</t>
+  </si>
+  <si>
+    <t>XIAOMIREDMI6A</t>
   </si>
   <si>
     <t>NOKIA</t>
@@ -544,7 +538,7 @@
     <t>GOOGLE</t>
   </si>
   <si>
-    <t>PIXEL3XL</t>
+    <t>GOOGLEPIXEL3XL</t>
   </si>
   <si>
     <t>ONEPLUS</t>
@@ -565,15 +559,173 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -634,8 +786,194 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -658,44 +996,320 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="41" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9"/>
+    <cellStyle name="Virgule" xfId="3" builtinId="3"/>
+    <cellStyle name="60 % - Accent6" xfId="4" builtinId="52"/>
+    <cellStyle name="Calcul" xfId="5" builtinId="22"/>
+    <cellStyle name="Titre" xfId="6" builtinId="15"/>
+    <cellStyle name="Monétaire [0]" xfId="7" builtinId="7"/>
+    <cellStyle name="Monétaire" xfId="8" builtinId="4"/>
+    <cellStyle name="Milliers [0]" xfId="9" builtinId="6"/>
+    <cellStyle name="Cellule liée" xfId="10" builtinId="24"/>
+    <cellStyle name="Pourcentage" xfId="11" builtinId="5"/>
+    <cellStyle name="Lien hypertexte" xfId="12" builtinId="8"/>
+    <cellStyle name="Avertissement" xfId="13" builtinId="11"/>
+    <cellStyle name="CTexte explicatif" xfId="14" builtinId="53"/>
+    <cellStyle name="Titre 1" xfId="15" builtinId="16"/>
+    <cellStyle name="Titre 2" xfId="16" builtinId="17"/>
+    <cellStyle name="Accent1" xfId="17" builtinId="29"/>
+    <cellStyle name="Titre 3" xfId="18" builtinId="18"/>
+    <cellStyle name="Accent2" xfId="19" builtinId="33"/>
+    <cellStyle name="Titre 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Neutre" xfId="21" builtinId="28"/>
+    <cellStyle name="Entrée" xfId="22" builtinId="20"/>
+    <cellStyle name="40 % - Accent2" xfId="23" builtinId="35"/>
+    <cellStyle name="Sortie" xfId="24" builtinId="21"/>
+    <cellStyle name="Vérification de cellule" xfId="25" builtinId="23"/>
+    <cellStyle name="Total" xfId="26" builtinId="25"/>
+    <cellStyle name="Accent4" xfId="27" builtinId="41"/>
+    <cellStyle name="Satisfaisant" xfId="28" builtinId="26"/>
+    <cellStyle name="Insatisfaisant" xfId="29" builtinId="27"/>
+    <cellStyle name="20 % - Accent1" xfId="30" builtinId="30"/>
+    <cellStyle name="40 % - Accent1" xfId="31" builtinId="31"/>
+    <cellStyle name="60 % - Accent1" xfId="32" builtinId="32"/>
+    <cellStyle name="20 % - Accent2" xfId="33" builtinId="34"/>
+    <cellStyle name="60 % - Accent2" xfId="34" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="35" builtinId="37"/>
+    <cellStyle name="20 % - Accent3" xfId="36" builtinId="38"/>
+    <cellStyle name="40 % - Accent3" xfId="37" builtinId="39"/>
+    <cellStyle name="60 % - Accent3" xfId="38" builtinId="40"/>
+    <cellStyle name="20 % - Accent4" xfId="39" builtinId="42"/>
+    <cellStyle name="40 % - Accent4" xfId="40" builtinId="43"/>
+    <cellStyle name="60 % - Accent4" xfId="41" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="42" builtinId="45"/>
+    <cellStyle name="20 % - Accent5" xfId="43" builtinId="46"/>
+    <cellStyle name="40 % - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60 % - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="20 % - Accent6" xfId="47" builtinId="50"/>
+    <cellStyle name="40 % - Accent6" xfId="48" builtinId="51"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -982,28 +1596,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170:D172"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="G183" sqref="G183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="35.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="19.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="19.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="19.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,1332 +1628,1332 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:4">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>210</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:4">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>35</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>145</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+    <row r="5" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>139</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="2:4">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>151</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="2:4">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>136</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="2:4">
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>136</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="2:4">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>142</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="2:4">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>151</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="2:4">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>115</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="2:4">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>123</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="2:4">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>123</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="2:4">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>120</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="2:4">
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>132</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="2:4">
+      <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="3">
         <v>132</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="2:4">
+      <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="3">
         <v>147</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="3">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="2:4">
+      <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="3">
         <v>147</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="3">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+    <row r="19" spans="2:4">
+      <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="3">
         <v>130</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="3">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="2:4">
+      <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>130</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="3">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="2:4">
+      <c r="B21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <v>151</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="3">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="2:4">
+      <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="3">
         <v>151</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="3">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+    <row r="23" spans="2:4">
+      <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="3">
         <v>107</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+    <row r="24" spans="2:4">
+      <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>117</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+    <row r="25" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="3">
         <v>117</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="26" ht="15.75" customHeight="1" spans="1:4">
+      <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="4">
         <v>134</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="4">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
+    <row r="27" spans="2:4">
+      <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="4">
         <v>135</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="4">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
+    <row r="28" spans="2:4">
+      <c r="B28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="4">
         <v>150</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="4">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+    <row r="29" spans="2:4">
+      <c r="B29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="4">
         <v>132</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="4">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+    <row r="30" spans="2:4">
+      <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="4">
         <v>141</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="4">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
+    <row r="31" spans="2:4">
+      <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="4">
         <v>140</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="4">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
+    <row r="32" spans="2:4">
+      <c r="B32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="4">
         <v>151</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="4">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+    <row r="33" spans="2:4">
+      <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="4">
         <v>140</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="4">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
+    <row r="34" spans="2:4">
+      <c r="B34" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="4">
         <v>149</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="4">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
+    <row r="35" spans="2:4">
+      <c r="B35" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="4">
         <v>140</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="4">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
+    <row r="36" spans="2:4">
+      <c r="B36" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="4">
         <v>130</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="4">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
+    <row r="37" spans="2:4">
+      <c r="B37" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="4">
         <v>148</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="4">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
+    <row r="38" spans="2:4">
+      <c r="B38" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="4">
         <v>120</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="4">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
+    <row r="39" spans="2:4">
+      <c r="B39" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="4">
         <v>130</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="4">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
+    <row r="40" spans="2:4">
+      <c r="B40" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="4">
         <v>128</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="4">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
+    <row r="41" spans="2:4">
+      <c r="B41" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="4">
         <v>131</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="4">
         <v>610</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
+    <row r="42" spans="2:4">
+      <c r="B42" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="4">
         <v>139</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="4">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
+    <row r="43" spans="2:4">
+      <c r="B43" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="4">
         <v>138</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="4">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="7" t="s">
+    <row r="44" spans="2:4">
+      <c r="B44" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="4">
         <v>152</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="4">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
+    <row r="45" spans="2:4">
+      <c r="B45" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="4">
         <v>138</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="4">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
+    <row r="46" spans="2:4">
+      <c r="B46" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="4">
         <v>148</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="4">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
+    <row r="47" spans="2:4">
+      <c r="B47" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="4">
         <v>141</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="4">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="6" t="s">
+    <row r="48" spans="2:4">
+      <c r="B48" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="4">
         <v>145</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="4">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="6" t="s">
+    <row r="49" spans="2:4">
+      <c r="B49" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="4">
         <v>149</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="4">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="6" t="s">
+    <row r="50" spans="2:4">
+      <c r="B50" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="4">
         <v>150</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="4">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="6" t="s">
+    <row r="51" spans="2:4">
+      <c r="B51" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="4">
         <v>150</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="4">
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="6" t="s">
+    <row r="52" spans="2:4">
+      <c r="B52" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="4">
         <v>141</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="4">
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="6" t="s">
+    <row r="53" spans="2:4">
+      <c r="B53" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="4">
         <v>151</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="4">
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="6" t="s">
+    <row r="54" spans="2:4">
+      <c r="B54" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="4">
         <v>155</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D54" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="6" t="s">
+    <row r="55" spans="2:4">
+      <c r="B55" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="4">
         <v>147</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D55" s="4">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="6" t="s">
+    <row r="56" spans="2:4">
+      <c r="B56" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="4">
         <v>152</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56" s="4">
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="6" t="s">
+    <row r="57" spans="2:4">
+      <c r="B57" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="4">
         <v>159</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
+    <row r="58" spans="2:4">
+      <c r="B58" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="4">
         <v>159</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="6" t="s">
+    <row r="59" spans="2:4">
+      <c r="B59" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="4">
         <v>147</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="4">
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="6" t="s">
+    <row r="60" spans="2:4">
+      <c r="B60" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="4">
         <v>140</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="4">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="6" t="s">
+    <row r="61" spans="2:4">
+      <c r="B61" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="4">
         <v>157</v>
       </c>
-      <c r="D61" s="7">
+      <c r="D61" s="4">
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="7" t="s">
+    <row r="62" spans="2:4">
+      <c r="B62" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="4">
         <v>162</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D62" s="4">
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="6" t="s">
+    <row r="63" spans="2:4">
+      <c r="B63" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="4">
         <v>155</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D63" s="4">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="7" t="s">
+    <row r="64" spans="2:4">
+      <c r="B64" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="4">
         <v>143</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64" s="4">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="7" t="s">
+    <row r="65" spans="2:4">
+      <c r="B65" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="4">
         <v>143</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="4">
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="6" t="s">
+    <row r="66" spans="2:4">
+      <c r="B66" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="4">
         <v>129</v>
       </c>
-      <c r="D66" s="7">
+      <c r="D66" s="4">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="6" t="s">
+    <row r="67" spans="2:4">
+      <c r="B67" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="4">
         <v>129</v>
       </c>
-      <c r="D67" s="7">
+      <c r="D67" s="4">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="6" t="s">
+    <row r="68" spans="2:4">
+      <c r="B68" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="4">
         <v>128</v>
       </c>
-      <c r="D68" s="7">
+      <c r="D68" s="4">
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="6" t="s">
+    <row r="69" spans="2:4">
+      <c r="B69" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="4">
         <v>136</v>
       </c>
-      <c r="D69" s="7">
+      <c r="D69" s="4">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="7" t="s">
+    <row r="70" spans="2:4">
+      <c r="B70" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="4">
         <v>143</v>
       </c>
-      <c r="D70" s="7">
+      <c r="D70" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="7" t="s">
+    <row r="71" spans="2:4">
+      <c r="B71" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="4">
         <v>151</v>
       </c>
-      <c r="D71" s="7">
+      <c r="D71" s="4">
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="6" t="s">
+    <row r="72" spans="2:4">
+      <c r="B72" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="4">
         <v>163</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D72" s="4">
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="6" t="s">
+    <row r="73" spans="2:4">
+      <c r="B73" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="4">
         <v>129</v>
       </c>
-      <c r="D73" s="7">
+      <c r="D73" s="4">
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="6" t="s">
+    <row r="74" spans="2:4">
+      <c r="B74" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="4">
         <v>129</v>
       </c>
-      <c r="D74" s="7">
+      <c r="D74" s="4">
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="6" t="s">
+    <row r="75" spans="2:4">
+      <c r="B75" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="4">
         <v>132</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D75" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="6" t="s">
+    <row r="76" spans="2:4">
+      <c r="B76" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C76" s="7">
+      <c r="C76" s="4">
         <v>138</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D76" s="4">
         <v>62</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="6" t="s">
+    <row r="77" spans="2:4">
+      <c r="B77" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="4">
         <v>137</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="4">
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="6" t="s">
+    <row r="78" spans="2:4">
+      <c r="B78" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C78" s="4">
         <v>152</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D78" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="6" t="s">
+    <row r="79" spans="2:4">
+      <c r="B79" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C79" s="4">
         <v>152</v>
       </c>
-      <c r="D79" s="7">
+      <c r="D79" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="6" t="s">
+    <row r="80" spans="2:4">
+      <c r="B80" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="4">
         <v>144</v>
       </c>
-      <c r="D80" s="7">
+      <c r="D80" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="6" t="s">
+    <row r="81" spans="2:4">
+      <c r="B81" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="4">
         <v>144</v>
       </c>
-      <c r="D81" s="7">
+      <c r="D81" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="6" t="s">
+    <row r="82" spans="2:4">
+      <c r="B82" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C82" s="4">
         <v>148</v>
       </c>
-      <c r="D82" s="7">
+      <c r="D82" s="4">
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="6" t="s">
+    <row r="83" spans="2:4">
+      <c r="B83" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="4">
         <v>146</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D83" s="4">
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="6" t="s">
+    <row r="84" spans="2:4">
+      <c r="B84" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="4">
         <v>150</v>
       </c>
-      <c r="D84" s="7">
+      <c r="D84" s="4">
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="20" t="s">
+    <row r="85" spans="2:4">
+      <c r="B85" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C85" s="4">
         <v>154</v>
       </c>
-      <c r="D85" s="7">
+      <c r="D85" s="4">
         <v>67</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="6" t="s">
+    <row r="86" spans="2:4">
+      <c r="B86" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C86" s="4">
         <v>153</v>
       </c>
-      <c r="D86" s="7">
+      <c r="D86" s="4">
         <v>68</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="6" t="s">
+    <row r="87" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B87" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C87" s="4">
         <v>147</v>
       </c>
-      <c r="D87" s="7">
+      <c r="D87" s="4">
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="6" t="s">
+    <row r="88" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B88" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C88" s="7">
+      <c r="C88" s="4">
         <v>157</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D88" s="4">
         <v>73</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="7" t="s">
+    <row r="89" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B89" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C89" s="7">
+      <c r="C89" s="4">
         <v>169</v>
       </c>
-      <c r="D89" s="7">
+      <c r="D89" s="4">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="6" t="s">
+    <row r="90" spans="2:4">
+      <c r="B90" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C90" s="4">
         <v>134</v>
       </c>
-      <c r="D90" s="7">
+      <c r="D90" s="4">
         <v>64</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
+    <row r="91" spans="1:4">
+      <c r="A91" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C91" s="9">
+      <c r="C91" s="5">
         <v>139</v>
       </c>
-      <c r="D91" s="9">
+      <c r="D91" s="5">
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="8" t="s">
+    <row r="92" spans="2:4">
+      <c r="B92" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C92" s="9">
+      <c r="C92" s="5">
         <v>139</v>
       </c>
-      <c r="D92" s="9">
+      <c r="D92" s="5">
         <v>66</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="8" t="s">
+    <row r="93" spans="2:4">
+      <c r="B93" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C93" s="5">
         <v>141</v>
       </c>
-      <c r="D93" s="9">
+      <c r="D93" s="5">
         <v>67</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="8" t="s">
+    <row r="94" spans="2:4">
+      <c r="B94" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="5">
         <v>134</v>
       </c>
-      <c r="D94" s="9">
+      <c r="D94" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="8" t="s">
+    <row r="95" spans="2:4">
+      <c r="B95" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C95" s="9">
+      <c r="C95" s="5">
         <v>139</v>
       </c>
-      <c r="D95" s="9">
+      <c r="D95" s="5">
         <v>65</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="8" t="s">
+    <row r="96" spans="2:4">
+      <c r="B96" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C96" s="9">
+      <c r="C96" s="5">
         <v>139</v>
       </c>
-      <c r="D96" s="9">
+      <c r="D96" s="5">
         <v>65</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="8" t="s">
+    <row r="97" spans="2:4">
+      <c r="B97" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C97" s="5">
         <v>138</v>
       </c>
-      <c r="D97" s="9">
+      <c r="D97" s="5">
         <v>63</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="8" t="s">
+    <row r="98" spans="2:4">
+      <c r="B98" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C98" s="9">
+      <c r="C98" s="5">
         <v>139</v>
       </c>
-      <c r="D98" s="9">
+      <c r="D98" s="5">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="8" t="s">
+    <row r="99" spans="2:4">
+      <c r="B99" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C99" s="9">
+      <c r="C99" s="5">
         <v>140</v>
       </c>
-      <c r="D99" s="9">
+      <c r="D99" s="5">
         <v>62</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="8" t="s">
+    <row r="100" spans="2:4">
+      <c r="B100" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C100" s="9">
+      <c r="C100" s="5">
         <v>148</v>
       </c>
-      <c r="D100" s="9">
+      <c r="D100" s="5">
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="8" t="s">
+    <row r="101" spans="2:4">
+      <c r="B101" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C101" s="9">
+      <c r="C101" s="5">
         <v>142</v>
       </c>
-      <c r="D101" s="9">
+      <c r="D101" s="5">
         <v>65</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="8" t="s">
+    <row r="102" spans="2:4">
+      <c r="B102" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C102" s="9">
+      <c r="C102" s="5">
         <v>139</v>
       </c>
-      <c r="D102" s="9">
+      <c r="D102" s="5">
         <v>63</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="8" t="s">
+    <row r="103" spans="2:4">
+      <c r="B103" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C103" s="9">
+      <c r="C103" s="5">
         <v>144</v>
       </c>
-      <c r="D103" s="9">
+      <c r="D103" s="5">
         <v>63</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="8" t="s">
+    <row r="104" spans="2:4">
+      <c r="B104" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C104" s="9">
+      <c r="C104" s="5">
         <v>142</v>
       </c>
-      <c r="D104" s="9">
+      <c r="D104" s="5">
         <v>63</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="8" t="s">
+    <row r="105" spans="2:4">
+      <c r="B105" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C105" s="9">
+      <c r="C105" s="5">
         <v>139</v>
       </c>
-      <c r="D105" s="9">
+      <c r="D105" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="8" t="s">
+    <row r="106" spans="2:4">
+      <c r="B106" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C106" s="9">
+      <c r="C106" s="5">
         <v>149</v>
       </c>
-      <c r="D106" s="9">
+      <c r="D106" s="5">
         <v>63</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="8" t="s">
+    <row r="107" spans="2:4">
+      <c r="B107" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C107" s="9">
+      <c r="C107" s="5">
         <v>159</v>
       </c>
-      <c r="D107" s="9">
+      <c r="D107" s="5">
         <v>83</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="8" t="s">
+    <row r="108" spans="2:4">
+      <c r="B108" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C108" s="9">
+      <c r="C108" s="5">
         <v>150</v>
       </c>
-      <c r="D108" s="9">
+      <c r="D108" s="5">
         <v>75</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="8" t="s">
+    <row r="109" spans="2:4">
+      <c r="B109" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C109" s="9">
+      <c r="C109" s="5">
         <v>140</v>
       </c>
-      <c r="D109" s="9">
+      <c r="D109" s="5">
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="8" t="s">
+    <row r="110" spans="2:4">
+      <c r="B110" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C110" s="9">
+      <c r="C110" s="5">
         <v>146</v>
       </c>
-      <c r="D110" s="9">
+      <c r="D110" s="5">
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="8" t="s">
+    <row r="111" spans="2:4">
+      <c r="B111" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C111" s="9">
+      <c r="C111" s="5">
         <v>148</v>
       </c>
-      <c r="D111" s="9">
+      <c r="D111" s="5">
         <v>67</v>
       </c>
     </row>
-    <row r="112" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="8" t="s">
+    <row r="112" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B112" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C112" s="9">
+      <c r="C112" s="5">
         <v>151</v>
       </c>
-      <c r="D112" s="9">
+      <c r="D112" s="5">
         <v>64</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="8" t="s">
+    <row r="113" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B113" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C113" s="9">
+      <c r="C113" s="5">
         <v>148</v>
       </c>
-      <c r="D113" s="9">
+      <c r="D113" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B114" s="8" t="s">
+    <row r="114" spans="2:4">
+      <c r="B114" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C114" s="9">
+      <c r="C114" s="5">
         <v>150</v>
       </c>
-      <c r="D114" s="9">
+      <c r="D114" s="5">
         <v>67</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B115" s="9" t="s">
+    <row r="115" spans="2:4">
+      <c r="B115" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C115" s="9">
+      <c r="C115" s="5">
         <v>142</v>
       </c>
-      <c r="D115" s="9">
+      <c r="D115" s="5">
         <v>68</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B116" s="9" t="s">
+    <row r="116" spans="2:4">
+      <c r="B116" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C116" s="9">
+      <c r="C116" s="5">
         <v>142</v>
       </c>
-      <c r="D116" s="9">
+      <c r="D116" s="5">
         <v>71</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B117" s="9" t="s">
+    <row r="117" spans="2:4">
+      <c r="B117" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C117" s="9">
+      <c r="C117" s="5">
         <v>144</v>
       </c>
-      <c r="D117" s="9">
+      <c r="D117" s="5">
         <v>73</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B118" s="9" t="s">
+    <row r="118" spans="2:4">
+      <c r="B118" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C118" s="9">
+      <c r="C118" s="5">
         <v>130</v>
       </c>
-      <c r="D118" s="9">
+      <c r="D118" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B119" s="8" t="s">
+    <row r="119" spans="2:4">
+      <c r="B119" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C119" s="9">
+      <c r="C119" s="5">
         <v>140</v>
       </c>
-      <c r="D119" s="9">
+      <c r="D119" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B120" s="8" t="s">
+    <row r="120" spans="2:4">
+      <c r="B120" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C120" s="9">
+      <c r="C120" s="5">
         <v>141</v>
       </c>
-      <c r="D120" s="9">
+      <c r="D120" s="5">
         <v>62</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="8" t="s">
+    <row r="121" spans="2:8">
+      <c r="B121" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C121" s="9">
+      <c r="C121" s="5">
         <v>164</v>
       </c>
-      <c r="D121" s="9">
+      <c r="D121" s="5">
         <v>81</v>
       </c>
       <c r="F121" t="s">
@@ -2352,557 +2966,556 @@
         <v>81</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="8" t="s">
+    <row r="122" spans="2:4">
+      <c r="B122" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C122" s="9">
+      <c r="C122" s="5">
         <v>163</v>
       </c>
-      <c r="D122" s="9">
+      <c r="D122" s="5">
         <v>75</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B123" s="8" t="s">
+    <row r="123" spans="2:4">
+      <c r="B123" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C123" s="9">
+      <c r="C123" s="5">
         <v>159</v>
       </c>
-      <c r="D123" s="9">
+      <c r="D123" s="5">
         <v>78</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="11" t="s">
+    <row r="124" spans="1:4">
+      <c r="A124" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B124" s="11" t="s">
+      <c r="B124" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C124" s="11">
+      <c r="C124" s="6">
         <v>153</v>
       </c>
-      <c r="D124" s="11">
+      <c r="D124" s="6">
         <v>79</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B125" s="11" t="s">
+    <row r="125" spans="2:4">
+      <c r="B125" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C125" s="11">
+      <c r="C125" s="6">
         <v>151</v>
       </c>
-      <c r="D125" s="11">
+      <c r="D125" s="6">
         <v>75</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="10" t="s">
+    <row r="126" spans="2:4">
+      <c r="B126" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C126" s="11">
+      <c r="C126" s="6">
         <v>135</v>
       </c>
-      <c r="D126" s="11">
+      <c r="D126" s="6">
         <v>66</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B127" s="11" t="s">
+    <row r="127" spans="2:4">
+      <c r="B127" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C127" s="11">
+      <c r="C127" s="6">
         <v>152</v>
       </c>
-      <c r="D127" s="11">
+      <c r="D127" s="6">
         <v>73</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B128" s="11" t="s">
+    <row r="128" spans="2:4">
+      <c r="B128" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C128" s="11">
+      <c r="C128" s="6">
         <v>150</v>
       </c>
-      <c r="D128" s="11">
+      <c r="D128" s="6">
         <v>72</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B129" s="10" t="s">
+    <row r="129" spans="2:4">
+      <c r="B129" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C129" s="11">
+      <c r="C129" s="6">
         <v>135</v>
       </c>
-      <c r="D129" s="11">
+      <c r="D129" s="6">
         <v>64</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B130" s="10" t="s">
+    <row r="130" spans="2:4">
+      <c r="B130" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C130" s="11">
+      <c r="C130" s="6">
         <v>138</v>
       </c>
-      <c r="D130" s="11">
+      <c r="D130" s="6">
         <v>64</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B131" s="10" t="s">
+    <row r="131" spans="2:4">
+      <c r="B131" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C131" s="11">
+      <c r="C131" s="6">
         <v>152</v>
       </c>
-      <c r="D131" s="11">
+      <c r="D131" s="6">
         <v>66</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B132" s="10" t="s">
+    <row r="132" spans="2:4">
+      <c r="B132" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C132" s="11">
+      <c r="C132" s="6">
         <v>138</v>
       </c>
-      <c r="D132" s="11">
+      <c r="D132" s="6">
         <v>67</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B133" s="11" t="s">
+    <row r="133" spans="2:4">
+      <c r="B133" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C133" s="11">
+      <c r="C133" s="6">
         <v>139</v>
       </c>
-      <c r="D133" s="11">
+      <c r="D133" s="6">
         <v>60</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="10" t="s">
+    <row r="134" spans="2:4">
+      <c r="B134" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C134" s="11">
+      <c r="C134" s="6">
         <v>140</v>
       </c>
-      <c r="D134" s="11">
+      <c r="D134" s="6">
         <v>61</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="10" t="s">
+    <row r="135" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B135" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C135" s="11">
+      <c r="C135" s="6">
         <v>150</v>
       </c>
-      <c r="D135" s="11">
+      <c r="D135" s="6">
         <v>63</v>
       </c>
-      <c r="G135" s="18"/>
-    </row>
-    <row r="136" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="19" t="s">
+    </row>
+    <row r="136" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B136" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C136" s="11">
+      <c r="C136" s="6">
         <v>140</v>
       </c>
-      <c r="D136" s="11">
+      <c r="D136" s="6">
         <v>70</v>
       </c>
-      <c r="G136" s="18"/>
-    </row>
-    <row r="137" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="11" t="s">
+    </row>
+    <row r="137" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B137" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C137" s="11">
+      <c r="C137" s="6">
         <v>159</v>
       </c>
-      <c r="D137" s="11">
+      <c r="D137" s="6">
         <v>77</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="10" t="s">
+    <row r="138" ht="15.75" customHeight="1" spans="2:4">
+      <c r="B138" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C138" s="11">
+      <c r="C138" s="6">
         <v>155</v>
       </c>
-      <c r="D138" s="11">
+      <c r="D138" s="6">
         <v>74</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="13" t="s">
+    <row r="139" spans="1:4">
+      <c r="A139" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B139" s="12" t="s">
+      <c r="B139" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C139" s="13">
+      <c r="C139" s="7">
         <v>145</v>
       </c>
-      <c r="D139" s="13">
+      <c r="D139" s="7">
         <v>64</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B140" s="12" t="s">
+    <row r="140" spans="2:4">
+      <c r="B140" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C140" s="13">
+      <c r="C140" s="7">
         <v>156</v>
       </c>
-      <c r="D140" s="13">
+      <c r="D140" s="7">
         <v>78</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B141" s="12" t="s">
+    <row r="141" spans="2:4">
+      <c r="B141" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C141" s="13">
+      <c r="C141" s="7">
         <v>152</v>
       </c>
-      <c r="D141" s="13">
+      <c r="D141" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B142" s="12" t="s">
+    <row r="142" spans="2:4">
+      <c r="B142" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C142" s="13">
+      <c r="C142" s="7">
         <v>137</v>
       </c>
-      <c r="D142" s="13">
+      <c r="D142" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="13" t="s">
+    <row r="143" spans="2:4">
+      <c r="B143" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C143" s="13">
+      <c r="C143" s="7">
         <v>145</v>
       </c>
-      <c r="D143" s="13">
+      <c r="D143" s="7">
         <v>72</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B144" s="12" t="s">
+    <row r="144" spans="2:4">
+      <c r="B144" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C144" s="13">
+      <c r="C144" s="7">
         <v>138</v>
       </c>
-      <c r="D144" s="13">
+      <c r="D144" s="7">
         <v>64</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="12" t="s">
+    <row r="145" spans="2:4">
+      <c r="B145" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C145" s="13">
+      <c r="C145" s="7">
         <v>137</v>
       </c>
-      <c r="D145" s="13">
+      <c r="D145" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="12" t="s">
+    <row r="146" spans="2:4">
+      <c r="B146" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C146" s="13">
+      <c r="C146" s="7">
         <v>138</v>
       </c>
-      <c r="D146" s="13">
+      <c r="D146" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="12" t="s">
+    <row r="147" spans="2:4">
+      <c r="B147" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C147" s="13">
+      <c r="C147" s="7">
         <v>160</v>
       </c>
-      <c r="D147" s="13">
+      <c r="D147" s="7">
         <v>71</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="12" t="s">
+    <row r="148" spans="2:4">
+      <c r="B148" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C148" s="13">
+      <c r="C148" s="7">
         <v>141</v>
       </c>
-      <c r="D148" s="13">
+      <c r="D148" s="7">
         <v>58</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="12" t="s">
+    <row r="149" spans="2:4">
+      <c r="B149" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C149" s="13">
+      <c r="C149" s="7">
         <v>160</v>
       </c>
-      <c r="D149" s="13">
+      <c r="D149" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="12" t="s">
+    <row r="150" spans="2:4">
+      <c r="B150" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C150" s="13">
+      <c r="C150" s="7">
         <v>160</v>
       </c>
-      <c r="D150" s="13">
+      <c r="D150" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="13" t="s">
+    <row r="151" spans="2:4">
+      <c r="B151" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C151" s="13">
+      <c r="C151" s="7">
         <v>168</v>
       </c>
-      <c r="D151" s="13">
+      <c r="D151" s="7">
         <v>82</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="12" t="s">
+    <row r="152" spans="2:4">
+      <c r="B152" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C152" s="13">
+      <c r="C152" s="7">
         <v>143</v>
       </c>
-      <c r="D152" s="13">
+      <c r="D152" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B153" s="12" t="s">
+    <row r="153" spans="2:4">
+      <c r="B153" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C153" s="13">
+      <c r="C153" s="7">
         <v>145</v>
       </c>
-      <c r="D153" s="13">
+      <c r="D153" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="12" t="s">
+    <row r="154" spans="2:4">
+      <c r="B154" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C154" s="13">
+      <c r="C154" s="7">
         <v>133</v>
       </c>
-      <c r="D154" s="13">
+      <c r="D154" s="7">
         <v>56</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="12" t="s">
+    <row r="155" spans="2:4">
+      <c r="B155" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C155" s="13">
+      <c r="C155" s="7">
         <v>141</v>
       </c>
-      <c r="D155" s="13">
+      <c r="D155" s="7">
         <v>55</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="12" t="s">
+    <row r="156" spans="2:4">
+      <c r="B156" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C156" s="13">
+      <c r="C156" s="7">
         <v>142</v>
       </c>
-      <c r="D156" s="13">
+      <c r="D156" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="12" t="s">
+    <row r="157" spans="2:4">
+      <c r="B157" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C157" s="13">
+      <c r="C157" s="7">
         <v>123</v>
       </c>
-      <c r="D157" s="13">
+      <c r="D157" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="12" t="s">
+    <row r="158" spans="2:4">
+      <c r="B158" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="C158" s="13">
+      <c r="C158" s="7">
         <v>160</v>
       </c>
-      <c r="D158" s="13">
+      <c r="D158" s="7">
         <v>80</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="14" t="s">
+    <row r="159" spans="1:4">
+      <c r="A159" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B159" s="14" t="s">
+      <c r="B159" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C159" s="14">
+      <c r="C159" s="2">
         <v>159</v>
       </c>
-      <c r="D159" s="14">
+      <c r="D159" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="14" t="s">
+    <row r="160" spans="2:4">
+      <c r="B160" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C160" s="14">
+      <c r="C160" s="2">
         <v>159</v>
       </c>
-      <c r="D160" s="14">
+      <c r="D160" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="14" t="s">
+    <row r="161" spans="2:4">
+      <c r="B161" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C161" s="14">
+      <c r="C161" s="2">
         <v>150</v>
       </c>
-      <c r="D161" s="14">
+      <c r="D161" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="14" t="s">
+    <row r="162" spans="2:4">
+      <c r="B162" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C162" s="14">
+      <c r="C162" s="2">
         <v>150</v>
       </c>
-      <c r="D162" s="14">
+      <c r="D162" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="15" t="s">
+    <row r="163" spans="1:4">
+      <c r="A163" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B163" s="15" t="s">
+      <c r="B163" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C163" s="15">
+      <c r="C163" s="8">
         <v>152</v>
       </c>
-      <c r="D163" s="15">
+      <c r="D163" s="8">
         <v>75</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="15" t="s">
+    <row r="164" spans="2:4">
+      <c r="B164" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C164" s="15">
+      <c r="C164" s="8">
         <v>147</v>
       </c>
-      <c r="D164" s="15">
+      <c r="D164" s="8">
         <v>75</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="16" t="s">
+    <row r="165" spans="1:4">
+      <c r="A165" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="B165" s="16" t="s">
+      <c r="B165" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C165" s="16">
+      <c r="C165" s="9">
         <v>160</v>
       </c>
-      <c r="D165" s="16">
+      <c r="D165" s="9">
         <v>80</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="17" t="s">
+    <row r="166" spans="1:4">
+      <c r="A166" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="B166" s="17" t="s">
+      <c r="B166" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C166" s="17">
+      <c r="C166" s="10">
         <v>155</v>
       </c>
-      <c r="D166" s="17">
+      <c r="D166" s="10">
         <v>75</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="17" t="s">
+    <row r="167" spans="2:4">
+      <c r="B167" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="C167" s="17">
+      <c r="C167" s="10">
         <v>157</v>
       </c>
-      <c r="D167" s="17">
+      <c r="D167" s="10">
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="17" t="s">
+    <row r="168" spans="2:4">
+      <c r="B168" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C168" s="17">
+      <c r="C168" s="10">
         <v>155</v>
       </c>
-      <c r="D168" s="17">
+      <c r="D168" s="10">
         <v>75</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="17" t="s">
+    <row r="169" spans="2:4">
+      <c r="B169" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C169" s="17">
+      <c r="C169" s="10">
         <v>159</v>
       </c>
-      <c r="D169" s="17">
+      <c r="D169" s="10">
         <v>77</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>